<commit_message>
Update German and Danish string resources. Adjust form settings controls to compensate for culture.
</commit_message>
<xml_diff>
--- a/ErgoLux/localization/Strings.xlsx
+++ b/ErgoLux/localization/Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfredoa\source\repos\ErgoLux\ErgoLux\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094531AE-8A5C-4A0A-8DB8-83A766644D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF8B46B-B679-4DA4-B57F-B786CADD8ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56FEE487-7C3D-43D6-8681-78DA792873A9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4254" uniqueCount="2919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4254" uniqueCount="2922">
   <si>
     <t>strBtnAccept</t>
   </si>
@@ -9147,6 +9147,15 @@
   <si>
     <t>Недопустимое имя строки идентификатора культуры._x000D_
 {0}</t>
+  </si>
+  <si>
+    <t>Schaubild</t>
+  </si>
+  <si>
+    <t>Grafik</t>
+  </si>
+  <si>
+    <t>Plots</t>
   </si>
 </sst>
 </file>
@@ -9299,8 +9308,8 @@
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{1595DE94-DACC-4C2E-A9FE-64A16CEEE124}" name="Name"/>
     <tableColumn id="2" xr3:uid="{CED3BB36-677C-40E9-BE52-77FF563954E9}" name="en"/>
-    <tableColumn id="3" xr3:uid="{615018CF-FF37-42D7-A961-D5DAFE57D5F8}" name="bn-BD" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{F3A69273-04AB-4EFF-92F7-EEC2A65EE476}" name="cs-CZ" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{615018CF-FF37-42D7-A961-D5DAFE57D5F8}" name="bn-BD" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{F3A69273-04AB-4EFF-92F7-EEC2A65EE476}" name="cs-CZ" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{30E82FEC-A598-4030-9696-90202D311F4F}" name="da-DK" dataDxfId="24"/>
     <tableColumn id="6" xr3:uid="{3BD77616-8009-49E8-BE45-26AF71142049}" name="de-DE" dataDxfId="23"/>
     <tableColumn id="7" xr3:uid="{9C91D2C5-6EC4-4B85-9E3A-02A9FF054E0E}" name="es-ES" dataDxfId="22"/>
@@ -9330,23 +9339,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2B9A328-18B0-4D97-8119-033E0C517499}" name="Tabla2" displayName="Tabla2" ref="A1:N130" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A2B9A328-18B0-4D97-8119-033E0C517499}" name="Tabla2" displayName="Tabla2" ref="A1:N130" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:N130" xr:uid="{A2B9A328-18B0-4D97-8119-033E0C517499}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{D330F886-2198-47FA-8B26-3B7AF827B284}" name="Name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{94743D3C-8DA2-4D7D-9B50-8D2D3D590BC8}" name="en" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{CF4CF549-AD05-4FC2-92F0-AC69B47BB2B8}" name="ar" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{FF5F89E8-1AFE-4CCA-A0B2-B60C656F0388}" name="bn-BD" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{AB799060-5CAB-408F-9DD7-0F34E7D887D8}" name="da-DK" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{9598F162-9119-479D-8860-500C76E9454D}" name="de-DE" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{775A12D7-9809-4E61-9E2E-8C8395EA3276}" name="es-ES" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{D4F076E5-4E8D-4BCA-A73A-BA9C197B3456}" name="hi-IN" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2FBFF86D-86FA-444D-90A8-51E1F01A62FC}" name="it-IT" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{34957AEF-DE3E-4DBF-9384-2CBD71FC3620}" name="lt-LT" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{7B64BCA9-924D-4030-A1F9-E6ED3D94EA71}" name="nb-NO" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{03F4A539-0705-41B4-A55D-11D216140EB3}" name="nl-BE" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{1C56DB1B-9970-4914-AA0B-C2DBA1897F67}" name="pt-BR" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{014022CC-2259-4B0D-9D6F-C6F774BCCCED}" name="ru-RU" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D330F886-2198-47FA-8B26-3B7AF827B284}" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{94743D3C-8DA2-4D7D-9B50-8D2D3D590BC8}" name="en" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CF4CF549-AD05-4FC2-92F0-AC69B47BB2B8}" name="ar" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{FF5F89E8-1AFE-4CCA-A0B2-B60C656F0388}" name="bn-BD" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{AB799060-5CAB-408F-9DD7-0F34E7D887D8}" name="da-DK" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{9598F162-9119-479D-8860-500C76E9454D}" name="de-DE" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{775A12D7-9809-4E61-9E2E-8C8395EA3276}" name="es-ES" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{D4F076E5-4E8D-4BCA-A73A-BA9C197B3456}" name="hi-IN" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{2FBFF86D-86FA-444D-90A8-51E1F01A62FC}" name="it-IT" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{34957AEF-DE3E-4DBF-9384-2CBD71FC3620}" name="lt-LT" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{7B64BCA9-924D-4030-A1F9-E6ED3D94EA71}" name="nb-NO" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{03F4A539-0705-41B4-A55D-11D216140EB3}" name="nl-BE" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{1C56DB1B-9970-4914-AA0B-C2DBA1897F67}" name="pt-BR" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{014022CC-2259-4B0D-9D6F-C6F774BCCCED}" name="ru-RU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9651,8 +9660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F4CEA3-9611-4ED5-B045-AD95FBF589BC}">
   <dimension ref="A1:N187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17363,7 +17372,7 @@
         <v>320</v>
       </c>
       <c r="B172" t="s">
-        <v>321</v>
+        <v>2921</v>
       </c>
       <c r="C172" t="s">
         <v>656</v>
@@ -17372,10 +17381,10 @@
         <v>1832</v>
       </c>
       <c r="E172" t="s">
-        <v>321</v>
+        <v>2920</v>
       </c>
       <c r="F172" t="s">
-        <v>862</v>
+        <v>2919</v>
       </c>
       <c r="G172" t="s">
         <v>966</v>

</xml_diff>